<commit_message>
parallel plus snr test
</commit_message>
<xml_diff>
--- a/algorithmes/request.xlsx
+++ b/algorithmes/request.xlsx
@@ -340,13 +340,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E2"/>
+  <dimension ref="A2:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>-1</v>
       </c>
@@ -361,6 +361,21 @@
       </c>
       <c r="E2">
         <v>-1</v>
+      </c>
+      <c r="F2">
+        <v>-1</v>
+      </c>
+      <c r="G2">
+        <v>-1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>-1</v>
+      </c>
+      <c r="J2">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>